<commit_message>
summary and update of the project README
</commit_message>
<xml_diff>
--- a/1_Protocol/1_2_pre_material/知情同意签名表_被试费报销单.xlsx
+++ b/1_Protocol/1_2_pre_material/知情同意签名表_被试费报销单.xlsx
@@ -5,19 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HW\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project\Experiment\Self_Prioritization_Expt\1_Protocol\1_2_pre_material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F7AFEA-6C35-4FAB-9948-EFA66C845821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C3F1C8-1A2B-4BE6-81CA-DB66E06D3ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="知情同意签名表" sheetId="1" r:id="rId1"/>
     <sheet name="被试费报销单" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>知情同意签名表</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -61,6 +60,22 @@
   </si>
   <si>
     <t>s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>知情同意书签字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据公开同意书签字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日期（年/月/日）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -68,7 +83,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -108,6 +123,15 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="等线"/>
       <family val="3"/>
@@ -163,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -182,11 +206,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -507,43 +534,43 @@
   </sheetPr>
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="77" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="77" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.90625" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" customWidth="1"/>
+    <col min="2" max="2" width="19.7265625" customWidth="1"/>
+    <col min="3" max="3" width="20.54296875" customWidth="1"/>
     <col min="4" max="4" width="24.1796875" customWidth="1"/>
     <col min="5" max="5" width="18.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>5</v>
+      <c r="B2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="23.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -833,7 +860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B8E0ADE-2791-4FC7-8846-B7947730D61C}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -847,16 +874,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="36.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">

</xml_diff>